<commit_message>
Add new excel import sheet
</commit_message>
<xml_diff>
--- a/files/2019-2020/Zaalschema 2019-2020 v1.xlsx
+++ b/files/2019-2020/Zaalschema 2019-2020 v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwin/Documents/ZOD/files/2019-2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwin/Projects/zod-zaalvoetbal/files/2019-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E95D65-2D1F-A748-8BD5-5CC399ACE3A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D851C933-F5B8-1F42-B82C-7A35F2AD894F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="460" windowWidth="32800" windowHeight="20540" tabRatio="833" firstSheet="4" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5620" yWindow="2160" windowWidth="32800" windowHeight="20540" tabRatio="833" firstSheet="4" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O13-A" sheetId="85" r:id="rId1"/>
@@ -1272,14 +1272,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1296,19 +1296,19 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -8495,7 +8495,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F27" sqref="F27"/>
+      <selection pane="topRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8569,31 +8569,31 @@
       <c r="Y1" s="287"/>
       <c r="Z1" s="287"/>
       <c r="AA1" s="7"/>
-      <c r="AB1" s="289" t="s">
+      <c r="AB1" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC1" s="296"/>
+      <c r="AC1" s="297"/>
       <c r="AD1" s="287"/>
       <c r="AE1" s="287"/>
       <c r="AF1" s="7"/>
-      <c r="AG1" s="290" t="s">
+      <c r="AG1" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" s="297"/>
+      <c r="AH1" s="299"/>
       <c r="AI1" s="287"/>
       <c r="AJ1" s="287"/>
       <c r="AK1" s="7"/>
-      <c r="AL1" s="298" t="s">
+      <c r="AL1" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM1" s="298"/>
+      <c r="AM1" s="289"/>
       <c r="AN1" s="287"/>
       <c r="AO1" s="287"/>
       <c r="AP1" s="7"/>
-      <c r="AQ1" s="299" t="s">
+      <c r="AQ1" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR1" s="299"/>
+      <c r="AR1" s="290"/>
       <c r="AS1" s="7"/>
       <c r="AT1" t="s">
         <v>14</v>
@@ -8606,69 +8606,69 @@
       <c r="B2" s="276"/>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
-      <c r="E2" s="288" t="s">
+      <c r="E2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F2" s="288"/>
+      <c r="F2" s="300"/>
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
       <c r="I2" s="22"/>
-      <c r="J2" s="288" t="s">
+      <c r="J2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="288"/>
+      <c r="K2" s="300"/>
       <c r="L2" s="22"/>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
-      <c r="O2" s="288" t="s">
+      <c r="O2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P2" s="288"/>
+      <c r="P2" s="300"/>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
       <c r="S2" s="22"/>
-      <c r="T2" s="288" t="s">
+      <c r="T2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U2" s="288"/>
+      <c r="U2" s="300"/>
       <c r="V2" s="22"/>
       <c r="W2" s="22"/>
       <c r="X2" s="22"/>
-      <c r="Y2" s="288" t="s">
+      <c r="Y2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z2" s="288"/>
+      <c r="Z2" s="300"/>
       <c r="AA2" s="22"/>
       <c r="AB2" s="22"/>
       <c r="AC2" s="22"/>
-      <c r="AD2" s="288" t="s">
+      <c r="AD2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE2" s="288"/>
+      <c r="AE2" s="300"/>
       <c r="AF2" s="22"/>
       <c r="AG2" s="22"/>
       <c r="AH2" s="22"/>
-      <c r="AI2" s="288" t="s">
+      <c r="AI2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ2" s="288"/>
+      <c r="AJ2" s="300"/>
       <c r="AK2" s="22"/>
       <c r="AL2" s="22"/>
       <c r="AM2" s="22"/>
-      <c r="AN2" s="288" t="s">
+      <c r="AN2" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO2" s="288"/>
+      <c r="AO2" s="300"/>
       <c r="AP2" s="22"/>
       <c r="AQ2" s="22"/>
       <c r="AR2" s="22"/>
       <c r="AS2" s="22"/>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A3" s="300">
+      <c r="A3" s="288">
         <v>0.375</v>
       </c>
-      <c r="B3" s="300">
+      <c r="B3" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C3" s="39"/>
@@ -8716,10 +8716,10 @@
       <c r="AS3" s="6"/>
     </row>
     <row r="4" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A4" s="300">
+      <c r="A4" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B4" s="300">
+      <c r="B4" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C4" s="39"/>
@@ -8767,10 +8767,10 @@
       <c r="AS4" s="6"/>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A5" s="300">
+      <c r="A5" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B5" s="300">
+      <c r="B5" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C5" s="39"/>
@@ -8818,10 +8818,10 @@
       <c r="AS5" s="6"/>
     </row>
     <row r="6" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A6" s="300">
+      <c r="A6" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B6" s="300">
+      <c r="B6" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C6" s="39"/>
@@ -8869,10 +8869,10 @@
       <c r="AS6" s="6"/>
     </row>
     <row r="7" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A7" s="300">
+      <c r="A7" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B7" s="300">
+      <c r="B7" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C7" s="39"/>
@@ -8920,10 +8920,10 @@
       <c r="AS7" s="6"/>
     </row>
     <row r="8" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A8" s="300">
+      <c r="A8" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B8" s="300">
+      <c r="B8" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C8" s="39"/>
@@ -8971,10 +8971,10 @@
       <c r="AS8" s="6"/>
     </row>
     <row r="9" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A9" s="300">
+      <c r="A9" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B9" s="300">
+      <c r="B9" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C9" s="39"/>
@@ -9022,10 +9022,10 @@
       <c r="AS9" s="6"/>
     </row>
     <row r="10" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A10" s="300">
+      <c r="A10" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B10" s="300">
+      <c r="B10" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C10" s="39"/>
@@ -9073,10 +9073,10 @@
       <c r="AS10" s="5"/>
     </row>
     <row r="11" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A11" s="300">
+      <c r="A11" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B11" s="300">
+      <c r="B11" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C11" s="39"/>
@@ -9124,10 +9124,10 @@
       <c r="AS11" s="5"/>
     </row>
     <row r="12" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A12" s="300">
+      <c r="A12" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B12" s="300">
+      <c r="B12" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C12" s="39"/>
@@ -9175,10 +9175,10 @@
       <c r="AS12" s="5"/>
     </row>
     <row r="13" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A13" s="300">
+      <c r="A13" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B13" s="300">
+      <c r="B13" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C13" s="18"/>
@@ -9226,10 +9226,10 @@
       <c r="AS13" s="5"/>
     </row>
     <row r="14" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A14" s="300">
+      <c r="A14" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B14" s="300">
+      <c r="B14" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C14" s="18"/>
@@ -9277,10 +9277,10 @@
       <c r="AS14" s="5"/>
     </row>
     <row r="15" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A15" s="300">
+      <c r="A15" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B15" s="300">
+      <c r="B15" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C15" s="18"/>
@@ -9328,10 +9328,10 @@
       <c r="AS15" s="5"/>
     </row>
     <row r="16" spans="1:46" x14ac:dyDescent="0.15">
-      <c r="A16" s="300">
+      <c r="A16" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B16" s="300">
+      <c r="B16" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C16" s="18"/>
@@ -9379,10 +9379,10 @@
       <c r="AS16" s="5"/>
     </row>
     <row r="17" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A17" s="300">
+      <c r="A17" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B17" s="300">
+      <c r="B17" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C17" s="18"/>
@@ -9430,10 +9430,10 @@
       <c r="AS17" s="5"/>
     </row>
     <row r="18" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A18" s="300">
+      <c r="A18" s="288">
         <v>0.625</v>
       </c>
-      <c r="B18" s="300">
+      <c r="B18" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C18" s="18"/>
@@ -9481,10 +9481,10 @@
       <c r="AS18" s="5"/>
     </row>
     <row r="19" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A19" s="300">
+      <c r="A19" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B19" s="300">
+      <c r="B19" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C19" s="18"/>
@@ -9532,10 +9532,10 @@
       <c r="AS19" s="5"/>
     </row>
     <row r="20" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A20" s="300">
+      <c r="A20" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B20" s="300">
+      <c r="B20" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C20" s="18"/>
@@ -9583,10 +9583,10 @@
       <c r="AS20" s="5"/>
     </row>
     <row r="21" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A21" s="300">
+      <c r="A21" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B21" s="300">
+      <c r="B21" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C21" s="18"/>
@@ -9634,10 +9634,10 @@
       <c r="AS21" s="5"/>
     </row>
     <row r="22" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A22" s="300">
+      <c r="A22" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B22" s="300">
+      <c r="B22" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C22" s="18"/>
@@ -9801,25 +9801,25 @@
       </c>
       <c r="X24" s="295"/>
       <c r="AA24" s="7"/>
-      <c r="AB24" s="289" t="s">
+      <c r="AB24" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC24" s="296"/>
+      <c r="AC24" s="297"/>
       <c r="AF24" s="7"/>
-      <c r="AG24" s="290" t="s">
+      <c r="AG24" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH24" s="297"/>
+      <c r="AH24" s="299"/>
       <c r="AK24" s="7"/>
-      <c r="AL24" s="298" t="s">
+      <c r="AL24" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM24" s="298"/>
+      <c r="AM24" s="289"/>
       <c r="AP24" s="7"/>
-      <c r="AQ24" s="299" t="s">
+      <c r="AQ24" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR24" s="299"/>
+      <c r="AR24" s="290"/>
       <c r="AS24" s="7"/>
     </row>
     <row r="25" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -9829,69 +9829,69 @@
       <c r="B25" s="278"/>
       <c r="C25" s="23"/>
       <c r="D25" s="23"/>
-      <c r="E25" s="288" t="s">
+      <c r="E25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F25" s="288"/>
+      <c r="F25" s="300"/>
       <c r="G25" s="23"/>
       <c r="H25" s="24"/>
       <c r="I25" s="24"/>
-      <c r="J25" s="288" t="s">
+      <c r="J25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K25" s="288"/>
+      <c r="K25" s="300"/>
       <c r="L25" s="23"/>
       <c r="M25" s="23"/>
       <c r="N25" s="23"/>
-      <c r="O25" s="288" t="s">
+      <c r="O25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P25" s="288"/>
+      <c r="P25" s="300"/>
       <c r="Q25" s="23"/>
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
-      <c r="T25" s="288" t="s">
+      <c r="T25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U25" s="288"/>
+      <c r="U25" s="300"/>
       <c r="V25" s="23"/>
       <c r="W25" s="23"/>
       <c r="X25" s="23"/>
-      <c r="Y25" s="288" t="s">
+      <c r="Y25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z25" s="288"/>
+      <c r="Z25" s="300"/>
       <c r="AA25" s="23"/>
       <c r="AB25" s="23"/>
       <c r="AC25" s="23"/>
-      <c r="AD25" s="288" t="s">
+      <c r="AD25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE25" s="288"/>
+      <c r="AE25" s="300"/>
       <c r="AF25" s="23"/>
       <c r="AG25" s="23"/>
       <c r="AH25" s="23"/>
-      <c r="AI25" s="288" t="s">
+      <c r="AI25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ25" s="288"/>
+      <c r="AJ25" s="300"/>
       <c r="AK25" s="23"/>
       <c r="AL25" s="23"/>
       <c r="AM25" s="23"/>
-      <c r="AN25" s="288" t="s">
+      <c r="AN25" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO25" s="288"/>
+      <c r="AO25" s="300"/>
       <c r="AP25" s="23"/>
       <c r="AQ25" s="23"/>
       <c r="AR25" s="23"/>
       <c r="AS25" s="23"/>
     </row>
     <row r="26" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A26" s="300">
+      <c r="A26" s="288">
         <v>0.375</v>
       </c>
-      <c r="B26" s="300">
+      <c r="B26" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C26" s="95" t="s">
@@ -9900,8 +9900,12 @@
       <c r="D26" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="284"/>
-      <c r="F26" s="284"/>
+      <c r="E26" s="284">
+        <v>4</v>
+      </c>
+      <c r="F26" s="284">
+        <v>3</v>
+      </c>
       <c r="G26" s="8"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>
@@ -9959,10 +9963,10 @@
       <c r="AS26" s="5"/>
     </row>
     <row r="27" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A27" s="300">
+      <c r="A27" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B27" s="300">
+      <c r="B27" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C27" s="95" t="s">
@@ -10030,10 +10034,10 @@
       <c r="AS27" s="5"/>
     </row>
     <row r="28" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A28" s="300">
+      <c r="A28" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B28" s="300">
+      <c r="B28" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C28" s="95" t="s">
@@ -10101,10 +10105,10 @@
       <c r="AS28" s="5"/>
     </row>
     <row r="29" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A29" s="300">
+      <c r="A29" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B29" s="300">
+      <c r="B29" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C29" s="95" t="s">
@@ -10172,10 +10176,10 @@
       <c r="AS29" s="5"/>
     </row>
     <row r="30" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A30" s="300">
+      <c r="A30" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B30" s="300">
+      <c r="B30" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C30" s="95" t="s">
@@ -10243,10 +10247,10 @@
       <c r="AS30" s="8"/>
     </row>
     <row r="31" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A31" s="300">
+      <c r="A31" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B31" s="300">
+      <c r="B31" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C31" s="113" t="s">
@@ -10314,10 +10318,10 @@
       <c r="AS31" s="8"/>
     </row>
     <row r="32" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A32" s="300">
+      <c r="A32" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B32" s="300">
+      <c r="B32" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C32" s="113" t="s">
@@ -10381,10 +10385,10 @@
       <c r="AS32" s="8"/>
     </row>
     <row r="33" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A33" s="300">
+      <c r="A33" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B33" s="300">
+      <c r="B33" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C33" s="113" t="s">
@@ -10448,10 +10452,10 @@
       <c r="AS33" s="8"/>
     </row>
     <row r="34" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A34" s="300">
+      <c r="A34" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B34" s="300">
+      <c r="B34" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C34" s="118" t="s">
@@ -10515,10 +10519,10 @@
       <c r="AS34" s="8"/>
     </row>
     <row r="35" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A35" s="300">
+      <c r="A35" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B35" s="300">
+      <c r="B35" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C35" s="118" t="s">
@@ -10582,10 +10586,10 @@
       <c r="AS35" s="8"/>
     </row>
     <row r="36" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A36" s="300">
+      <c r="A36" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B36" s="300">
+      <c r="B36" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C36" s="6"/>
@@ -10641,10 +10645,10 @@
       <c r="AS36" s="8"/>
     </row>
     <row r="37" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A37" s="300">
+      <c r="A37" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B37" s="300">
+      <c r="B37" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C37" s="6"/>
@@ -10700,10 +10704,10 @@
       <c r="AS37" s="8"/>
     </row>
     <row r="38" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A38" s="300">
+      <c r="A38" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B38" s="300">
+      <c r="B38" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C38" s="6"/>
@@ -10755,10 +10759,10 @@
       <c r="AS38" s="8"/>
     </row>
     <row r="39" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A39" s="300">
+      <c r="A39" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B39" s="300">
+      <c r="B39" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C39" s="6"/>
@@ -10810,10 +10814,10 @@
       <c r="AS39" s="8"/>
     </row>
     <row r="40" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A40" s="300">
+      <c r="A40" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B40" s="300">
+      <c r="B40" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C40" s="6"/>
@@ -10865,10 +10869,10 @@
       <c r="AS40" s="5"/>
     </row>
     <row r="41" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A41" s="300">
+      <c r="A41" s="288">
         <v>0.625</v>
       </c>
-      <c r="B41" s="300">
+      <c r="B41" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C41" s="8"/>
@@ -10916,10 +10920,10 @@
       <c r="AS41" s="5"/>
     </row>
     <row r="42" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A42" s="300">
+      <c r="A42" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B42" s="300">
+      <c r="B42" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C42" s="8"/>
@@ -10967,10 +10971,10 @@
       <c r="AS42" s="5"/>
     </row>
     <row r="43" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A43" s="300">
+      <c r="A43" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B43" s="300">
+      <c r="B43" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C43" s="8"/>
@@ -11018,10 +11022,10 @@
       <c r="AS43" s="5"/>
     </row>
     <row r="44" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A44" s="300">
+      <c r="A44" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B44" s="300">
+      <c r="B44" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C44" s="8"/>
@@ -11069,10 +11073,10 @@
       <c r="AS44" s="5"/>
     </row>
     <row r="45" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A45" s="300">
+      <c r="A45" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B45" s="300">
+      <c r="B45" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C45" s="8"/>
@@ -11248,25 +11252,25 @@
       </c>
       <c r="X47" s="295"/>
       <c r="AA47" s="7"/>
-      <c r="AB47" s="289" t="s">
+      <c r="AB47" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC47" s="296"/>
+      <c r="AC47" s="297"/>
       <c r="AF47" s="7"/>
-      <c r="AG47" s="290" t="s">
+      <c r="AG47" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH47" s="297"/>
+      <c r="AH47" s="299"/>
       <c r="AK47" s="7"/>
-      <c r="AL47" s="298" t="s">
+      <c r="AL47" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM47" s="298"/>
+      <c r="AM47" s="289"/>
       <c r="AP47" s="7"/>
-      <c r="AQ47" s="299" t="s">
+      <c r="AQ47" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR47" s="299"/>
+      <c r="AR47" s="290"/>
       <c r="AS47" s="7"/>
     </row>
     <row r="48" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -11276,69 +11280,69 @@
       <c r="B48" s="279"/>
       <c r="C48" s="23"/>
       <c r="D48" s="23"/>
-      <c r="E48" s="288" t="s">
+      <c r="E48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F48" s="288"/>
+      <c r="F48" s="300"/>
       <c r="G48" s="23"/>
       <c r="H48" s="25"/>
       <c r="I48" s="25"/>
-      <c r="J48" s="288" t="s">
+      <c r="J48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K48" s="288"/>
+      <c r="K48" s="300"/>
       <c r="L48" s="23"/>
       <c r="M48" s="25"/>
       <c r="N48" s="25"/>
-      <c r="O48" s="288" t="s">
+      <c r="O48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P48" s="288"/>
+      <c r="P48" s="300"/>
       <c r="Q48" s="23"/>
       <c r="R48" s="23"/>
       <c r="S48" s="23"/>
-      <c r="T48" s="288" t="s">
+      <c r="T48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U48" s="288"/>
+      <c r="U48" s="300"/>
       <c r="V48" s="23"/>
       <c r="W48" s="23"/>
       <c r="X48" s="23"/>
-      <c r="Y48" s="288" t="s">
+      <c r="Y48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z48" s="288"/>
+      <c r="Z48" s="300"/>
       <c r="AA48" s="23"/>
       <c r="AB48" s="23"/>
       <c r="AC48" s="23"/>
-      <c r="AD48" s="288" t="s">
+      <c r="AD48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE48" s="288"/>
+      <c r="AE48" s="300"/>
       <c r="AF48" s="23"/>
       <c r="AG48" s="23"/>
       <c r="AH48" s="23"/>
-      <c r="AI48" s="288" t="s">
+      <c r="AI48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ48" s="288"/>
+      <c r="AJ48" s="300"/>
       <c r="AK48" s="23"/>
       <c r="AL48" s="25"/>
       <c r="AM48" s="25"/>
-      <c r="AN48" s="288" t="s">
+      <c r="AN48" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO48" s="288"/>
+      <c r="AO48" s="300"/>
       <c r="AP48" s="23"/>
       <c r="AQ48" s="25"/>
       <c r="AR48" s="25"/>
       <c r="AS48" s="25"/>
     </row>
     <row r="49" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A49" s="300">
+      <c r="A49" s="288">
         <v>0.375</v>
       </c>
-      <c r="B49" s="300">
+      <c r="B49" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C49" s="184" t="s">
@@ -11406,10 +11410,10 @@
       <c r="AS49" s="5"/>
     </row>
     <row r="50" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A50" s="300">
+      <c r="A50" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B50" s="300">
+      <c r="B50" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C50" s="184" t="s">
@@ -11477,10 +11481,10 @@
       <c r="AS50" s="5"/>
     </row>
     <row r="51" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A51" s="300">
+      <c r="A51" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B51" s="300">
+      <c r="B51" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C51" s="184" t="s">
@@ -11548,10 +11552,10 @@
       <c r="AS51" s="5"/>
     </row>
     <row r="52" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A52" s="300">
+      <c r="A52" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B52" s="300">
+      <c r="B52" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C52" s="184" t="s">
@@ -11619,10 +11623,10 @@
       <c r="AS52" s="5"/>
     </row>
     <row r="53" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A53" s="300">
+      <c r="A53" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B53" s="300">
+      <c r="B53" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C53" s="184" t="s">
@@ -11690,10 +11694,10 @@
       <c r="AS53" s="8"/>
     </row>
     <row r="54" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A54" s="300">
+      <c r="A54" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B54" s="300">
+      <c r="B54" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C54" s="184" t="s">
@@ -11765,10 +11769,10 @@
       <c r="AS54" s="8"/>
     </row>
     <row r="55" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A55" s="300">
+      <c r="A55" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B55" s="300">
+      <c r="B55" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C55" s="186" t="s">
@@ -11840,10 +11844,10 @@
       <c r="AS55" s="8"/>
     </row>
     <row r="56" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A56" s="300">
+      <c r="A56" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B56" s="300">
+      <c r="B56" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C56" s="186" t="s">
@@ -11915,10 +11919,10 @@
       <c r="AS56" s="8"/>
     </row>
     <row r="57" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A57" s="300">
+      <c r="A57" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B57" s="300">
+      <c r="B57" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C57" s="187" t="s">
@@ -11990,10 +11994,10 @@
       <c r="AS57" s="8"/>
     </row>
     <row r="58" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A58" s="300">
+      <c r="A58" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B58" s="300">
+      <c r="B58" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C58" s="187" t="s">
@@ -12065,10 +12069,10 @@
       <c r="AS58" s="8"/>
     </row>
     <row r="59" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A59" s="300">
+      <c r="A59" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B59" s="300">
+      <c r="B59" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C59" s="6"/>
@@ -12128,10 +12132,10 @@
       <c r="AS59" s="8"/>
     </row>
     <row r="60" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A60" s="300">
+      <c r="A60" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B60" s="300">
+      <c r="B60" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C60" s="6"/>
@@ -12191,10 +12195,10 @@
       <c r="AS60" s="8"/>
     </row>
     <row r="61" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A61" s="300">
+      <c r="A61" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B61" s="300">
+      <c r="B61" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C61" s="6"/>
@@ -12254,10 +12258,10 @@
       <c r="AS61" s="8"/>
     </row>
     <row r="62" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A62" s="300">
+      <c r="A62" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B62" s="300">
+      <c r="B62" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C62" s="6"/>
@@ -12317,10 +12321,10 @@
       <c r="AS62" s="8"/>
     </row>
     <row r="63" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A63" s="300">
+      <c r="A63" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B63" s="300">
+      <c r="B63" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C63" s="6"/>
@@ -12380,10 +12384,10 @@
       <c r="AS63" s="5"/>
     </row>
     <row r="64" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A64" s="300">
+      <c r="A64" s="288">
         <v>0.625</v>
       </c>
-      <c r="B64" s="300">
+      <c r="B64" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C64" s="8"/>
@@ -12443,10 +12447,10 @@
       <c r="AS64" s="5"/>
     </row>
     <row r="65" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A65" s="300">
+      <c r="A65" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B65" s="300">
+      <c r="B65" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C65" s="8"/>
@@ -12506,10 +12510,10 @@
       <c r="AS65" s="5"/>
     </row>
     <row r="66" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A66" s="300">
+      <c r="A66" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B66" s="300">
+      <c r="B66" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C66" s="8"/>
@@ -12569,10 +12573,10 @@
       <c r="AS66" s="5"/>
     </row>
     <row r="67" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A67" s="300">
+      <c r="A67" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B67" s="300">
+      <c r="B67" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C67" s="8"/>
@@ -12632,10 +12636,10 @@
       <c r="AS67" s="5"/>
     </row>
     <row r="68" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A68" s="300">
+      <c r="A68" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B68" s="300">
+      <c r="B68" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C68" s="8"/>
@@ -12813,25 +12817,25 @@
       </c>
       <c r="X70" s="295"/>
       <c r="AA70" s="7"/>
-      <c r="AB70" s="289" t="s">
+      <c r="AB70" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC70" s="296"/>
+      <c r="AC70" s="297"/>
       <c r="AF70" s="7"/>
-      <c r="AG70" s="290" t="s">
+      <c r="AG70" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH70" s="297"/>
+      <c r="AH70" s="299"/>
       <c r="AK70" s="7"/>
-      <c r="AL70" s="298" t="s">
+      <c r="AL70" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM70" s="298"/>
+      <c r="AM70" s="289"/>
       <c r="AP70" s="7"/>
-      <c r="AQ70" s="299" t="s">
+      <c r="AQ70" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR70" s="299"/>
+      <c r="AR70" s="290"/>
       <c r="AS70" s="7"/>
     </row>
     <row r="71" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -12841,69 +12845,69 @@
       <c r="B71" s="278"/>
       <c r="C71" s="23"/>
       <c r="D71" s="23"/>
-      <c r="E71" s="288" t="s">
+      <c r="E71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F71" s="288"/>
+      <c r="F71" s="300"/>
       <c r="G71" s="23"/>
       <c r="H71" s="25"/>
       <c r="I71" s="25"/>
-      <c r="J71" s="288" t="s">
+      <c r="J71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K71" s="288"/>
+      <c r="K71" s="300"/>
       <c r="L71" s="23"/>
       <c r="M71" s="23"/>
       <c r="N71" s="23"/>
-      <c r="O71" s="288" t="s">
+      <c r="O71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P71" s="288"/>
+      <c r="P71" s="300"/>
       <c r="Q71" s="23"/>
       <c r="R71" s="23"/>
       <c r="S71" s="23"/>
-      <c r="T71" s="288" t="s">
+      <c r="T71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U71" s="288"/>
+      <c r="U71" s="300"/>
       <c r="V71" s="23"/>
       <c r="W71" s="23"/>
       <c r="X71" s="23"/>
-      <c r="Y71" s="288" t="s">
+      <c r="Y71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z71" s="288"/>
+      <c r="Z71" s="300"/>
       <c r="AA71" s="23"/>
       <c r="AB71" s="23"/>
       <c r="AC71" s="23"/>
-      <c r="AD71" s="288" t="s">
+      <c r="AD71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE71" s="288"/>
+      <c r="AE71" s="300"/>
       <c r="AF71" s="23"/>
       <c r="AG71" s="23"/>
       <c r="AH71" s="23"/>
-      <c r="AI71" s="288" t="s">
+      <c r="AI71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ71" s="288"/>
+      <c r="AJ71" s="300"/>
       <c r="AK71" s="23"/>
       <c r="AL71" s="23"/>
       <c r="AM71" s="23"/>
-      <c r="AN71" s="288" t="s">
+      <c r="AN71" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO71" s="288"/>
+      <c r="AO71" s="300"/>
       <c r="AP71" s="23"/>
       <c r="AQ71" s="23"/>
       <c r="AR71" s="23"/>
       <c r="AS71" s="23"/>
     </row>
     <row r="72" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A72" s="300">
+      <c r="A72" s="288">
         <v>0.375</v>
       </c>
-      <c r="B72" s="300">
+      <c r="B72" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C72" s="190" t="s">
@@ -12975,10 +12979,10 @@
       <c r="AS72" s="8"/>
     </row>
     <row r="73" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A73" s="300">
+      <c r="A73" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B73" s="300">
+      <c r="B73" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C73" s="190" t="s">
@@ -13050,10 +13054,10 @@
       <c r="AS73" s="8"/>
     </row>
     <row r="74" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A74" s="300">
+      <c r="A74" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B74" s="300">
+      <c r="B74" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C74" s="190" t="s">
@@ -13125,10 +13129,10 @@
       <c r="AS74" s="8"/>
     </row>
     <row r="75" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A75" s="300">
+      <c r="A75" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B75" s="300">
+      <c r="B75" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C75" s="190" t="s">
@@ -13200,10 +13204,10 @@
       <c r="AS75" s="8"/>
     </row>
     <row r="76" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A76" s="300">
+      <c r="A76" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B76" s="300">
+      <c r="B76" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C76" s="190" t="s">
@@ -13275,10 +13279,10 @@
       <c r="AS76" s="5"/>
     </row>
     <row r="77" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A77" s="300">
+      <c r="A77" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B77" s="300">
+      <c r="B77" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C77" s="270" t="s">
@@ -13350,10 +13354,10 @@
       <c r="AS77" s="6"/>
     </row>
     <row r="78" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A78" s="300">
+      <c r="A78" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B78" s="300">
+      <c r="B78" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C78" s="270" t="s">
@@ -13425,10 +13429,10 @@
       <c r="AS78" s="6"/>
     </row>
     <row r="79" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A79" s="300">
+      <c r="A79" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B79" s="300">
+      <c r="B79" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C79" s="270" t="s">
@@ -13500,10 +13504,10 @@
       <c r="AS79" s="6"/>
     </row>
     <row r="80" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A80" s="300">
+      <c r="A80" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B80" s="300">
+      <c r="B80" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C80" s="270" t="s">
@@ -13575,10 +13579,10 @@
       <c r="AS80" s="6"/>
     </row>
     <row r="81" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A81" s="300">
+      <c r="A81" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B81" s="300">
+      <c r="B81" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C81" s="270" t="s">
@@ -13646,10 +13650,10 @@
       <c r="AS81" s="6"/>
     </row>
     <row r="82" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A82" s="300">
+      <c r="A82" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B82" s="300">
+      <c r="B82" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C82" s="8"/>
@@ -13709,10 +13713,10 @@
       <c r="AS82" s="5"/>
     </row>
     <row r="83" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A83" s="300">
+      <c r="A83" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B83" s="300">
+      <c r="B83" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C83" s="8"/>
@@ -13772,10 +13776,10 @@
       <c r="AS83" s="5"/>
     </row>
     <row r="84" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A84" s="300">
+      <c r="A84" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B84" s="300">
+      <c r="B84" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C84" s="8"/>
@@ -13835,10 +13839,10 @@
       <c r="AS84" s="5"/>
     </row>
     <row r="85" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A85" s="300">
+      <c r="A85" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B85" s="300">
+      <c r="B85" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C85" s="8"/>
@@ -13898,10 +13902,10 @@
       <c r="AS85" s="5"/>
     </row>
     <row r="86" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A86" s="300">
+      <c r="A86" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B86" s="300">
+      <c r="B86" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C86" s="5"/>
@@ -13961,10 +13965,10 @@
       <c r="AS86" s="5"/>
     </row>
     <row r="87" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A87" s="300">
+      <c r="A87" s="288">
         <v>0.625</v>
       </c>
-      <c r="B87" s="300">
+      <c r="B87" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C87" s="5"/>
@@ -14024,10 +14028,10 @@
       <c r="AS87" s="6"/>
     </row>
     <row r="88" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A88" s="300">
+      <c r="A88" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B88" s="300">
+      <c r="B88" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C88" s="5"/>
@@ -14083,10 +14087,10 @@
       <c r="AS88" s="6"/>
     </row>
     <row r="89" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A89" s="300">
+      <c r="A89" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B89" s="300">
+      <c r="B89" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C89" s="5"/>
@@ -14142,10 +14146,10 @@
       <c r="AS89" s="6"/>
     </row>
     <row r="90" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A90" s="300">
+      <c r="A90" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B90" s="300">
+      <c r="B90" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C90" s="5"/>
@@ -14201,10 +14205,10 @@
       <c r="AS90" s="6"/>
     </row>
     <row r="91" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A91" s="300">
+      <c r="A91" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B91" s="300">
+      <c r="B91" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C91" s="5"/>
@@ -14382,25 +14386,25 @@
       </c>
       <c r="X93" s="295"/>
       <c r="AA93" s="7"/>
-      <c r="AB93" s="289" t="s">
+      <c r="AB93" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC93" s="296"/>
+      <c r="AC93" s="297"/>
       <c r="AF93" s="7"/>
-      <c r="AG93" s="290" t="s">
+      <c r="AG93" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH93" s="297"/>
+      <c r="AH93" s="299"/>
       <c r="AK93" s="7"/>
-      <c r="AL93" s="298" t="s">
+      <c r="AL93" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM93" s="298"/>
+      <c r="AM93" s="289"/>
       <c r="AP93" s="7"/>
-      <c r="AQ93" s="299" t="s">
+      <c r="AQ93" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR93" s="299"/>
+      <c r="AR93" s="290"/>
       <c r="AS93" s="7"/>
     </row>
     <row r="94" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -14410,69 +14414,69 @@
       <c r="B94" s="278"/>
       <c r="C94" s="25"/>
       <c r="D94" s="25"/>
-      <c r="E94" s="288" t="s">
+      <c r="E94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F94" s="288"/>
+      <c r="F94" s="300"/>
       <c r="G94" s="24"/>
       <c r="H94" s="24"/>
       <c r="I94" s="24"/>
-      <c r="J94" s="288" t="s">
+      <c r="J94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K94" s="288"/>
+      <c r="K94" s="300"/>
       <c r="L94" s="24"/>
       <c r="M94" s="24"/>
       <c r="N94" s="24"/>
-      <c r="O94" s="288" t="s">
+      <c r="O94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P94" s="288"/>
+      <c r="P94" s="300"/>
       <c r="Q94" s="24"/>
       <c r="R94" s="24"/>
       <c r="S94" s="24"/>
-      <c r="T94" s="288" t="s">
+      <c r="T94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U94" s="288"/>
+      <c r="U94" s="300"/>
       <c r="V94" s="24"/>
       <c r="W94" s="24"/>
       <c r="X94" s="24"/>
-      <c r="Y94" s="288" t="s">
+      <c r="Y94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z94" s="288"/>
+      <c r="Z94" s="300"/>
       <c r="AA94" s="24"/>
       <c r="AB94" s="24"/>
       <c r="AC94" s="24"/>
-      <c r="AD94" s="288" t="s">
+      <c r="AD94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE94" s="288"/>
+      <c r="AE94" s="300"/>
       <c r="AF94" s="24"/>
       <c r="AG94" s="24"/>
       <c r="AH94" s="24"/>
-      <c r="AI94" s="288" t="s">
+      <c r="AI94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ94" s="288"/>
+      <c r="AJ94" s="300"/>
       <c r="AK94" s="24"/>
       <c r="AL94" s="24"/>
       <c r="AM94" s="24"/>
-      <c r="AN94" s="288" t="s">
+      <c r="AN94" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO94" s="288"/>
+      <c r="AO94" s="300"/>
       <c r="AP94" s="24"/>
       <c r="AQ94" s="24"/>
       <c r="AR94" s="24"/>
       <c r="AS94" s="24"/>
     </row>
     <row r="95" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A95" s="300">
+      <c r="A95" s="288">
         <v>0.375</v>
       </c>
-      <c r="B95" s="300">
+      <c r="B95" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C95" s="37"/>
@@ -14548,10 +14552,10 @@
       <c r="AS95" s="4"/>
     </row>
     <row r="96" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A96" s="300">
+      <c r="A96" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B96" s="300">
+      <c r="B96" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C96" s="37"/>
@@ -14627,10 +14631,10 @@
       <c r="AS96" s="4"/>
     </row>
     <row r="97" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A97" s="300">
+      <c r="A97" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B97" s="300">
+      <c r="B97" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C97" s="37"/>
@@ -14706,10 +14710,10 @@
       <c r="AS97" s="4"/>
     </row>
     <row r="98" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A98" s="300">
+      <c r="A98" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B98" s="300">
+      <c r="B98" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C98" s="37"/>
@@ -14785,10 +14789,10 @@
       <c r="AS98" s="4"/>
     </row>
     <row r="99" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A99" s="300">
+      <c r="A99" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B99" s="300">
+      <c r="B99" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C99" s="37"/>
@@ -14864,10 +14868,10 @@
       <c r="AS99" s="6"/>
     </row>
     <row r="100" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A100" s="300">
+      <c r="A100" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B100" s="300">
+      <c r="B100" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C100" s="37"/>
@@ -14943,10 +14947,10 @@
       <c r="AS100" s="6"/>
     </row>
     <row r="101" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A101" s="300">
+      <c r="A101" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B101" s="300">
+      <c r="B101" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C101" s="37"/>
@@ -15022,10 +15026,10 @@
       <c r="AS101" s="6"/>
     </row>
     <row r="102" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A102" s="300">
+      <c r="A102" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B102" s="300">
+      <c r="B102" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C102" s="37"/>
@@ -15101,10 +15105,10 @@
       <c r="AS102" s="6"/>
     </row>
     <row r="103" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A103" s="300">
+      <c r="A103" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B103" s="300">
+      <c r="B103" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C103" s="37"/>
@@ -15180,10 +15184,10 @@
       <c r="AS103" s="6"/>
     </row>
     <row r="104" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A104" s="300">
+      <c r="A104" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B104" s="300">
+      <c r="B104" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C104" s="37"/>
@@ -15259,10 +15263,10 @@
       <c r="AS104" s="6"/>
     </row>
     <row r="105" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A105" s="300">
+      <c r="A105" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B105" s="300">
+      <c r="B105" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C105" s="37"/>
@@ -15322,10 +15326,10 @@
       <c r="AS105" s="6"/>
     </row>
     <row r="106" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A106" s="300">
+      <c r="A106" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B106" s="300">
+      <c r="B106" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C106" s="37"/>
@@ -15385,10 +15389,10 @@
       <c r="AS106" s="6"/>
     </row>
     <row r="107" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A107" s="300">
+      <c r="A107" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B107" s="300">
+      <c r="B107" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C107" s="37"/>
@@ -15448,10 +15452,10 @@
       <c r="AS107" s="6"/>
     </row>
     <row r="108" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A108" s="300">
+      <c r="A108" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B108" s="300">
+      <c r="B108" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C108" s="37"/>
@@ -15511,10 +15515,10 @@
       <c r="AS108" s="6"/>
     </row>
     <row r="109" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A109" s="300">
+      <c r="A109" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B109" s="300">
+      <c r="B109" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C109" s="37"/>
@@ -15574,10 +15578,10 @@
       <c r="AS109" s="4"/>
     </row>
     <row r="110" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A110" s="300">
+      <c r="A110" s="288">
         <v>0.625</v>
       </c>
-      <c r="B110" s="300">
+      <c r="B110" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C110" s="37"/>
@@ -15633,10 +15637,10 @@
       <c r="AS110" s="4"/>
     </row>
     <row r="111" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A111" s="300">
+      <c r="A111" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B111" s="300">
+      <c r="B111" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C111" s="37"/>
@@ -15692,10 +15696,10 @@
       <c r="AS111" s="4"/>
     </row>
     <row r="112" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A112" s="300">
+      <c r="A112" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B112" s="300">
+      <c r="B112" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C112" s="37"/>
@@ -15751,10 +15755,10 @@
       <c r="AS112" s="4"/>
     </row>
     <row r="113" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A113" s="300">
+      <c r="A113" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B113" s="300">
+      <c r="B113" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C113" s="37"/>
@@ -15810,10 +15814,10 @@
       <c r="AS113" s="6"/>
     </row>
     <row r="114" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A114" s="300">
+      <c r="A114" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B114" s="300">
+      <c r="B114" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C114" s="37"/>
@@ -15997,25 +16001,25 @@
       </c>
       <c r="X116" s="295"/>
       <c r="AA116" s="7"/>
-      <c r="AB116" s="289" t="s">
+      <c r="AB116" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC116" s="296"/>
+      <c r="AC116" s="297"/>
       <c r="AF116" s="7"/>
-      <c r="AG116" s="290" t="s">
+      <c r="AG116" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH116" s="297"/>
+      <c r="AH116" s="299"/>
       <c r="AK116" s="7"/>
-      <c r="AL116" s="298" t="s">
+      <c r="AL116" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM116" s="298"/>
+      <c r="AM116" s="289"/>
       <c r="AP116" s="7"/>
-      <c r="AQ116" s="299" t="s">
+      <c r="AQ116" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR116" s="299"/>
+      <c r="AR116" s="290"/>
       <c r="AS116" s="7"/>
     </row>
     <row r="117" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -16025,69 +16029,69 @@
       <c r="B117" s="278"/>
       <c r="C117" s="24"/>
       <c r="D117" s="24"/>
-      <c r="E117" s="288" t="s">
+      <c r="E117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F117" s="288"/>
+      <c r="F117" s="300"/>
       <c r="G117" s="24"/>
       <c r="H117" s="24"/>
       <c r="I117" s="24"/>
-      <c r="J117" s="288" t="s">
+      <c r="J117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K117" s="288"/>
+      <c r="K117" s="300"/>
       <c r="L117" s="24"/>
       <c r="M117" s="24"/>
       <c r="N117" s="24"/>
-      <c r="O117" s="288" t="s">
+      <c r="O117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P117" s="288"/>
+      <c r="P117" s="300"/>
       <c r="Q117" s="24"/>
       <c r="R117" s="24"/>
       <c r="S117" s="24"/>
-      <c r="T117" s="288" t="s">
+      <c r="T117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U117" s="288"/>
+      <c r="U117" s="300"/>
       <c r="V117" s="24"/>
       <c r="W117" s="24"/>
       <c r="X117" s="24"/>
-      <c r="Y117" s="288" t="s">
+      <c r="Y117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z117" s="288"/>
+      <c r="Z117" s="300"/>
       <c r="AA117" s="24"/>
       <c r="AB117" s="24"/>
       <c r="AC117" s="24"/>
-      <c r="AD117" s="288" t="s">
+      <c r="AD117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE117" s="288"/>
+      <c r="AE117" s="300"/>
       <c r="AF117" s="24"/>
       <c r="AG117" s="24"/>
       <c r="AH117" s="24"/>
-      <c r="AI117" s="288" t="s">
+      <c r="AI117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ117" s="288"/>
+      <c r="AJ117" s="300"/>
       <c r="AK117" s="24"/>
       <c r="AL117" s="24"/>
       <c r="AM117" s="24"/>
-      <c r="AN117" s="288" t="s">
+      <c r="AN117" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO117" s="288"/>
+      <c r="AO117" s="300"/>
       <c r="AP117" s="24"/>
       <c r="AQ117" s="24"/>
       <c r="AR117" s="24"/>
       <c r="AS117" s="24"/>
     </row>
     <row r="118" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A118" s="300">
+      <c r="A118" s="288">
         <v>0.375</v>
       </c>
-      <c r="B118" s="300">
+      <c r="B118" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C118" s="184" t="s">
@@ -16167,10 +16171,10 @@
       <c r="AS118" s="5"/>
     </row>
     <row r="119" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A119" s="300">
+      <c r="A119" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B119" s="300">
+      <c r="B119" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C119" s="184" t="s">
@@ -16250,10 +16254,10 @@
       <c r="AS119" s="5"/>
     </row>
     <row r="120" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A120" s="300">
+      <c r="A120" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B120" s="300">
+      <c r="B120" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C120" s="184" t="s">
@@ -16333,10 +16337,10 @@
       <c r="AS120" s="5"/>
     </row>
     <row r="121" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A121" s="300">
+      <c r="A121" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B121" s="300">
+      <c r="B121" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C121" s="184" t="s">
@@ -16416,10 +16420,10 @@
       <c r="AS121" s="5"/>
     </row>
     <row r="122" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A122" s="300">
+      <c r="A122" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B122" s="300">
+      <c r="B122" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C122" s="272" t="s">
@@ -16499,10 +16503,10 @@
       <c r="AS122" s="5"/>
     </row>
     <row r="123" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A123" s="300">
+      <c r="A123" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B123" s="300">
+      <c r="B123" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C123" s="272" t="s">
@@ -16578,10 +16582,10 @@
       <c r="AS123" s="5"/>
     </row>
     <row r="124" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A124" s="300">
+      <c r="A124" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B124" s="300">
+      <c r="B124" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C124" s="272" t="s">
@@ -16657,10 +16661,10 @@
       <c r="AS124" s="6"/>
     </row>
     <row r="125" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A125" s="300">
+      <c r="A125" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B125" s="300">
+      <c r="B125" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C125" s="273" t="s">
@@ -16736,10 +16740,10 @@
       <c r="AS125" s="6"/>
     </row>
     <row r="126" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A126" s="300">
+      <c r="A126" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B126" s="300">
+      <c r="B126" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C126" s="273" t="s">
@@ -16811,10 +16815,10 @@
       <c r="AS126" s="6"/>
     </row>
     <row r="127" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A127" s="300">
+      <c r="A127" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B127" s="300">
+      <c r="B127" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C127" s="38"/>
@@ -16882,10 +16886,10 @@
       <c r="AS127" s="6"/>
     </row>
     <row r="128" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A128" s="300">
+      <c r="A128" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B128" s="300">
+      <c r="B128" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C128" s="4"/>
@@ -16949,10 +16953,10 @@
       <c r="AS128" s="6"/>
     </row>
     <row r="129" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A129" s="300">
+      <c r="A129" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B129" s="300">
+      <c r="B129" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C129" s="4"/>
@@ -17016,10 +17020,10 @@
       <c r="AS129" s="6"/>
     </row>
     <row r="130" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A130" s="300">
+      <c r="A130" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B130" s="300">
+      <c r="B130" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C130" s="4"/>
@@ -17083,10 +17087,10 @@
       <c r="AS130" s="6"/>
     </row>
     <row r="131" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A131" s="300">
+      <c r="A131" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B131" s="300">
+      <c r="B131" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C131" s="4"/>
@@ -17146,10 +17150,10 @@
       <c r="AS131" s="6"/>
     </row>
     <row r="132" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A132" s="300">
+      <c r="A132" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B132" s="300">
+      <c r="B132" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C132" s="4"/>
@@ -17209,10 +17213,10 @@
       <c r="AS132" s="6"/>
     </row>
     <row r="133" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A133" s="300">
+      <c r="A133" s="288">
         <v>0.625</v>
       </c>
-      <c r="B133" s="300">
+      <c r="B133" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C133" s="4"/>
@@ -17268,10 +17272,10 @@
       <c r="AS133" s="6"/>
     </row>
     <row r="134" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A134" s="300">
+      <c r="A134" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B134" s="300">
+      <c r="B134" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C134" s="4"/>
@@ -17327,10 +17331,10 @@
       <c r="AS134" s="6"/>
     </row>
     <row r="135" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A135" s="300">
+      <c r="A135" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B135" s="300">
+      <c r="B135" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C135" s="4"/>
@@ -17386,10 +17390,10 @@
       <c r="AS135" s="6"/>
     </row>
     <row r="136" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A136" s="300">
+      <c r="A136" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B136" s="300">
+      <c r="B136" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C136" s="4"/>
@@ -17445,10 +17449,10 @@
       <c r="AS136" s="6"/>
     </row>
     <row r="137" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A137" s="300">
+      <c r="A137" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B137" s="300">
+      <c r="B137" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C137" s="4"/>
@@ -17628,25 +17632,25 @@
       </c>
       <c r="X139" s="295"/>
       <c r="AA139" s="7"/>
-      <c r="AB139" s="289" t="s">
+      <c r="AB139" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC139" s="296"/>
+      <c r="AC139" s="297"/>
       <c r="AF139" s="7"/>
-      <c r="AG139" s="290" t="s">
+      <c r="AG139" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH139" s="297"/>
+      <c r="AH139" s="299"/>
       <c r="AK139" s="7"/>
-      <c r="AL139" s="298" t="s">
+      <c r="AL139" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM139" s="298"/>
+      <c r="AM139" s="289"/>
       <c r="AP139" s="7"/>
-      <c r="AQ139" s="299" t="s">
+      <c r="AQ139" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR139" s="299"/>
+      <c r="AR139" s="290"/>
       <c r="AS139" s="7"/>
     </row>
     <row r="140" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -17656,69 +17660,69 @@
       <c r="B140" s="278"/>
       <c r="C140" s="26"/>
       <c r="D140" s="26"/>
-      <c r="E140" s="288" t="s">
+      <c r="E140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F140" s="288"/>
+      <c r="F140" s="300"/>
       <c r="G140" s="26"/>
       <c r="H140" s="24"/>
       <c r="I140" s="24"/>
-      <c r="J140" s="288" t="s">
+      <c r="J140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K140" s="288"/>
+      <c r="K140" s="300"/>
       <c r="L140" s="26"/>
       <c r="M140" s="24"/>
       <c r="N140" s="24"/>
-      <c r="O140" s="288" t="s">
+      <c r="O140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P140" s="288"/>
+      <c r="P140" s="300"/>
       <c r="Q140" s="26"/>
       <c r="R140" s="26"/>
       <c r="S140" s="26"/>
-      <c r="T140" s="288" t="s">
+      <c r="T140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U140" s="288"/>
+      <c r="U140" s="300"/>
       <c r="V140" s="26"/>
       <c r="W140" s="26"/>
       <c r="X140" s="26"/>
-      <c r="Y140" s="288" t="s">
+      <c r="Y140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z140" s="288"/>
+      <c r="Z140" s="300"/>
       <c r="AA140" s="26"/>
       <c r="AB140" s="26"/>
       <c r="AC140" s="26"/>
-      <c r="AD140" s="288" t="s">
+      <c r="AD140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE140" s="288"/>
+      <c r="AE140" s="300"/>
       <c r="AF140" s="26"/>
       <c r="AG140" s="26"/>
       <c r="AH140" s="26"/>
-      <c r="AI140" s="288" t="s">
+      <c r="AI140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ140" s="288"/>
+      <c r="AJ140" s="300"/>
       <c r="AK140" s="26"/>
       <c r="AL140" s="24"/>
       <c r="AM140" s="24"/>
-      <c r="AN140" s="288" t="s">
+      <c r="AN140" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO140" s="288"/>
+      <c r="AO140" s="300"/>
       <c r="AP140" s="26"/>
       <c r="AQ140" s="24"/>
       <c r="AR140" s="24"/>
       <c r="AS140" s="24"/>
     </row>
     <row r="141" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A141" s="300">
+      <c r="A141" s="288">
         <v>0.375</v>
       </c>
-      <c r="B141" s="300">
+      <c r="B141" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C141" s="6"/>
@@ -17790,10 +17794,10 @@
       <c r="AS141" s="6"/>
     </row>
     <row r="142" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A142" s="300">
+      <c r="A142" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B142" s="300">
+      <c r="B142" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C142" s="6"/>
@@ -17865,10 +17869,10 @@
       <c r="AS142" s="6"/>
     </row>
     <row r="143" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A143" s="300">
+      <c r="A143" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B143" s="300">
+      <c r="B143" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C143" s="6"/>
@@ -17940,10 +17944,10 @@
       <c r="AS143" s="6"/>
     </row>
     <row r="144" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A144" s="300">
+      <c r="A144" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B144" s="300">
+      <c r="B144" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C144" s="6"/>
@@ -18015,10 +18019,10 @@
       <c r="AS144" s="6"/>
     </row>
     <row r="145" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A145" s="300">
+      <c r="A145" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B145" s="300">
+      <c r="B145" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C145" s="4"/>
@@ -18090,10 +18094,10 @@
       <c r="AS145" s="6"/>
     </row>
     <row r="146" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A146" s="300">
+      <c r="A146" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B146" s="300">
+      <c r="B146" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C146" s="6"/>
@@ -18165,10 +18169,10 @@
       <c r="AS146" s="6"/>
     </row>
     <row r="147" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A147" s="300">
+      <c r="A147" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B147" s="300">
+      <c r="B147" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C147" s="6"/>
@@ -18236,10 +18240,10 @@
       <c r="AS147" s="6"/>
     </row>
     <row r="148" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A148" s="300">
+      <c r="A148" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B148" s="300">
+      <c r="B148" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C148" s="6"/>
@@ -18307,10 +18311,10 @@
       <c r="AS148" s="6"/>
     </row>
     <row r="149" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A149" s="300">
+      <c r="A149" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B149" s="300">
+      <c r="B149" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C149" s="6"/>
@@ -18378,10 +18382,10 @@
       <c r="AS149" s="6"/>
     </row>
     <row r="150" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A150" s="300">
+      <c r="A150" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B150" s="300">
+      <c r="B150" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C150" s="4"/>
@@ -18445,10 +18449,10 @@
       <c r="AS150" s="6"/>
     </row>
     <row r="151" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A151" s="300">
+      <c r="A151" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B151" s="300">
+      <c r="B151" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C151" s="4"/>
@@ -18508,10 +18512,10 @@
       <c r="AS151" s="6"/>
     </row>
     <row r="152" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A152" s="300">
+      <c r="A152" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B152" s="300">
+      <c r="B152" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C152" s="6"/>
@@ -18571,10 +18575,10 @@
       <c r="AS152" s="6"/>
     </row>
     <row r="153" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A153" s="300">
+      <c r="A153" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B153" s="300">
+      <c r="B153" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C153" s="6"/>
@@ -18634,10 +18638,10 @@
       <c r="AS153" s="6"/>
     </row>
     <row r="154" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A154" s="300">
+      <c r="A154" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B154" s="300">
+      <c r="B154" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C154" s="6"/>
@@ -18697,10 +18701,10 @@
       <c r="AS154" s="6"/>
     </row>
     <row r="155" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A155" s="300">
+      <c r="A155" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B155" s="300">
+      <c r="B155" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C155" s="6"/>
@@ -18760,10 +18764,10 @@
       <c r="AS155" s="6"/>
     </row>
     <row r="156" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A156" s="300">
+      <c r="A156" s="288">
         <v>0.625</v>
       </c>
-      <c r="B156" s="300">
+      <c r="B156" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C156" s="6"/>
@@ -18823,10 +18827,10 @@
       <c r="AS156" s="6"/>
     </row>
     <row r="157" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A157" s="300">
+      <c r="A157" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B157" s="300">
+      <c r="B157" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C157" s="4"/>
@@ -18886,10 +18890,10 @@
       <c r="AS157" s="6"/>
     </row>
     <row r="158" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A158" s="300">
+      <c r="A158" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B158" s="300">
+      <c r="B158" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C158" s="4"/>
@@ -18945,10 +18949,10 @@
       <c r="AS158" s="6"/>
     </row>
     <row r="159" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A159" s="300">
+      <c r="A159" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B159" s="300">
+      <c r="B159" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C159" s="4"/>
@@ -19000,10 +19004,10 @@
       <c r="AS159" s="6"/>
     </row>
     <row r="160" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A160" s="300">
+      <c r="A160" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B160" s="300">
+      <c r="B160" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C160" s="4"/>
@@ -19177,25 +19181,25 @@
       </c>
       <c r="X162" s="295"/>
       <c r="AA162" s="7"/>
-      <c r="AB162" s="289" t="s">
+      <c r="AB162" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC162" s="296"/>
+      <c r="AC162" s="297"/>
       <c r="AF162" s="7"/>
-      <c r="AG162" s="290" t="s">
+      <c r="AG162" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH162" s="297"/>
+      <c r="AH162" s="299"/>
       <c r="AK162" s="7"/>
-      <c r="AL162" s="298" t="s">
+      <c r="AL162" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM162" s="298"/>
+      <c r="AM162" s="289"/>
       <c r="AP162" s="7"/>
-      <c r="AQ162" s="299" t="s">
+      <c r="AQ162" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR162" s="299"/>
+      <c r="AR162" s="290"/>
       <c r="AS162" s="7"/>
     </row>
     <row r="163" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -19205,69 +19209,69 @@
       <c r="B163" s="278"/>
       <c r="C163" s="26"/>
       <c r="D163" s="26"/>
-      <c r="E163" s="288" t="s">
+      <c r="E163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F163" s="288"/>
+      <c r="F163" s="300"/>
       <c r="G163" s="26"/>
       <c r="H163" s="24"/>
       <c r="I163" s="24"/>
-      <c r="J163" s="288" t="s">
+      <c r="J163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K163" s="288"/>
+      <c r="K163" s="300"/>
       <c r="L163" s="26"/>
       <c r="M163" s="24"/>
       <c r="N163" s="24"/>
-      <c r="O163" s="288" t="s">
+      <c r="O163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P163" s="288"/>
+      <c r="P163" s="300"/>
       <c r="Q163" s="26"/>
       <c r="R163" s="26"/>
       <c r="S163" s="26"/>
-      <c r="T163" s="288" t="s">
+      <c r="T163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U163" s="288"/>
+      <c r="U163" s="300"/>
       <c r="V163" s="26"/>
       <c r="W163" s="26"/>
       <c r="X163" s="26"/>
-      <c r="Y163" s="288" t="s">
+      <c r="Y163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z163" s="288"/>
+      <c r="Z163" s="300"/>
       <c r="AA163" s="26"/>
       <c r="AB163" s="26"/>
       <c r="AC163" s="26"/>
-      <c r="AD163" s="288" t="s">
+      <c r="AD163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE163" s="288"/>
+      <c r="AE163" s="300"/>
       <c r="AF163" s="26"/>
       <c r="AG163" s="26"/>
       <c r="AH163" s="26"/>
-      <c r="AI163" s="288" t="s">
+      <c r="AI163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ163" s="288"/>
+      <c r="AJ163" s="300"/>
       <c r="AK163" s="26"/>
       <c r="AL163" s="24"/>
       <c r="AM163" s="24"/>
-      <c r="AN163" s="288" t="s">
+      <c r="AN163" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO163" s="288"/>
+      <c r="AO163" s="300"/>
       <c r="AP163" s="26"/>
       <c r="AQ163" s="24"/>
       <c r="AR163" s="24"/>
       <c r="AS163" s="24"/>
     </row>
     <row r="164" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A164" s="300">
+      <c r="A164" s="288">
         <v>0.375</v>
       </c>
-      <c r="B164" s="300">
+      <c r="B164" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C164" s="6"/>
@@ -19327,10 +19331,10 @@
       <c r="AS164" s="4"/>
     </row>
     <row r="165" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A165" s="300">
+      <c r="A165" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B165" s="300">
+      <c r="B165" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C165" s="6"/>
@@ -19390,10 +19394,10 @@
       <c r="AS165" s="4"/>
     </row>
     <row r="166" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A166" s="300">
+      <c r="A166" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B166" s="300">
+      <c r="B166" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C166" s="6"/>
@@ -19453,10 +19457,10 @@
       <c r="AS166" s="6"/>
     </row>
     <row r="167" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A167" s="300">
+      <c r="A167" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B167" s="300">
+      <c r="B167" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C167" s="6"/>
@@ -19516,10 +19520,10 @@
       <c r="AS167" s="6"/>
     </row>
     <row r="168" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A168" s="300">
+      <c r="A168" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B168" s="300">
+      <c r="B168" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C168" s="4"/>
@@ -19579,10 +19583,10 @@
       <c r="AS168" s="6"/>
     </row>
     <row r="169" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A169" s="300">
+      <c r="A169" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B169" s="300">
+      <c r="B169" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C169" s="4"/>
@@ -19642,10 +19646,10 @@
       <c r="AS169" s="6"/>
     </row>
     <row r="170" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A170" s="300">
+      <c r="A170" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B170" s="300">
+      <c r="B170" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C170" s="4"/>
@@ -19697,10 +19701,10 @@
       <c r="AS170" s="6"/>
     </row>
     <row r="171" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A171" s="300">
+      <c r="A171" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B171" s="300">
+      <c r="B171" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C171" s="4"/>
@@ -19752,10 +19756,10 @@
       <c r="AS171" s="6"/>
     </row>
     <row r="172" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A172" s="300">
+      <c r="A172" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B172" s="300">
+      <c r="B172" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C172" s="4"/>
@@ -19807,10 +19811,10 @@
       <c r="AS172" s="6"/>
     </row>
     <row r="173" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A173" s="300">
+      <c r="A173" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B173" s="300">
+      <c r="B173" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C173" s="4"/>
@@ -19862,10 +19866,10 @@
       <c r="AS173" s="6"/>
     </row>
     <row r="174" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A174" s="300">
+      <c r="A174" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B174" s="300">
+      <c r="B174" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C174" s="4"/>
@@ -19917,10 +19921,10 @@
       <c r="AS174" s="6"/>
     </row>
     <row r="175" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A175" s="300">
+      <c r="A175" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B175" s="300">
+      <c r="B175" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C175" s="4"/>
@@ -19972,10 +19976,10 @@
       <c r="AS175" s="6"/>
     </row>
     <row r="176" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A176" s="300">
+      <c r="A176" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B176" s="300">
+      <c r="B176" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C176" s="4"/>
@@ -20023,10 +20027,10 @@
       <c r="AS176" s="6"/>
     </row>
     <row r="177" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A177" s="300">
+      <c r="A177" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B177" s="300">
+      <c r="B177" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C177" s="4"/>
@@ -20074,10 +20078,10 @@
       <c r="AS177" s="6"/>
     </row>
     <row r="178" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A178" s="300">
+      <c r="A178" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B178" s="300">
+      <c r="B178" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C178" s="4"/>
@@ -20125,10 +20129,10 @@
       <c r="AS178" s="6"/>
     </row>
     <row r="179" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A179" s="300">
+      <c r="A179" s="288">
         <v>0.625</v>
       </c>
-      <c r="B179" s="300">
+      <c r="B179" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C179" s="4"/>
@@ -20176,10 +20180,10 @@
       <c r="AS179" s="6"/>
     </row>
     <row r="180" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A180" s="300">
+      <c r="A180" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B180" s="300">
+      <c r="B180" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C180" s="4"/>
@@ -20227,10 +20231,10 @@
       <c r="AS180" s="6"/>
     </row>
     <row r="181" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A181" s="300">
+      <c r="A181" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B181" s="300">
+      <c r="B181" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C181" s="4"/>
@@ -20278,10 +20282,10 @@
       <c r="AS181" s="6"/>
     </row>
     <row r="182" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A182" s="300">
+      <c r="A182" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B182" s="300">
+      <c r="B182" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C182" s="4"/>
@@ -20329,10 +20333,10 @@
       <c r="AS182" s="6"/>
     </row>
     <row r="183" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A183" s="300">
+      <c r="A183" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B183" s="300">
+      <c r="B183" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C183" s="4"/>
@@ -20496,25 +20500,25 @@
       </c>
       <c r="X185" s="295"/>
       <c r="AA185" s="7"/>
-      <c r="AB185" s="289" t="s">
+      <c r="AB185" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC185" s="296"/>
+      <c r="AC185" s="297"/>
       <c r="AF185" s="7"/>
-      <c r="AG185" s="290" t="s">
+      <c r="AG185" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH185" s="297"/>
+      <c r="AH185" s="299"/>
       <c r="AK185" s="7"/>
-      <c r="AL185" s="298" t="s">
+      <c r="AL185" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM185" s="298"/>
+      <c r="AM185" s="289"/>
       <c r="AP185" s="7"/>
-      <c r="AQ185" s="299" t="s">
+      <c r="AQ185" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR185" s="299"/>
+      <c r="AR185" s="290"/>
       <c r="AS185" s="7"/>
     </row>
     <row r="186" spans="1:47" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -20524,69 +20528,69 @@
       <c r="B186" s="278"/>
       <c r="C186" s="24"/>
       <c r="D186" s="24"/>
-      <c r="E186" s="288" t="s">
+      <c r="E186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F186" s="288"/>
+      <c r="F186" s="300"/>
       <c r="G186" s="24"/>
       <c r="H186" s="24"/>
       <c r="I186" s="24"/>
-      <c r="J186" s="288" t="s">
+      <c r="J186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K186" s="288"/>
+      <c r="K186" s="300"/>
       <c r="L186" s="24"/>
       <c r="M186" s="26"/>
       <c r="N186" s="26"/>
-      <c r="O186" s="288" t="s">
+      <c r="O186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P186" s="288"/>
+      <c r="P186" s="300"/>
       <c r="Q186" s="24"/>
       <c r="R186" s="24"/>
       <c r="S186" s="24"/>
-      <c r="T186" s="288" t="s">
+      <c r="T186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U186" s="288"/>
+      <c r="U186" s="300"/>
       <c r="V186" s="24"/>
       <c r="W186" s="24"/>
       <c r="X186" s="24"/>
-      <c r="Y186" s="288" t="s">
+      <c r="Y186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z186" s="288"/>
+      <c r="Z186" s="300"/>
       <c r="AA186" s="24"/>
       <c r="AB186" s="24"/>
       <c r="AC186" s="24"/>
-      <c r="AD186" s="288" t="s">
+      <c r="AD186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE186" s="288"/>
+      <c r="AE186" s="300"/>
       <c r="AF186" s="24"/>
       <c r="AG186" s="24"/>
       <c r="AH186" s="24"/>
-      <c r="AI186" s="288" t="s">
+      <c r="AI186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ186" s="288"/>
+      <c r="AJ186" s="300"/>
       <c r="AK186" s="24"/>
       <c r="AL186" s="26"/>
       <c r="AM186" s="26"/>
-      <c r="AN186" s="288" t="s">
+      <c r="AN186" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO186" s="288"/>
+      <c r="AO186" s="300"/>
       <c r="AP186" s="24"/>
       <c r="AQ186" s="26"/>
       <c r="AR186" s="26"/>
       <c r="AS186" s="26"/>
     </row>
     <row r="187" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A187" s="300">
+      <c r="A187" s="288">
         <v>0.375</v>
       </c>
-      <c r="B187" s="300">
+      <c r="B187" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C187" s="6"/>
@@ -20634,10 +20638,10 @@
       <c r="AS187" s="6"/>
     </row>
     <row r="188" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A188" s="300">
+      <c r="A188" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B188" s="300">
+      <c r="B188" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C188" s="6"/>
@@ -20685,10 +20689,10 @@
       <c r="AS188" s="6"/>
     </row>
     <row r="189" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A189" s="300">
+      <c r="A189" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B189" s="300">
+      <c r="B189" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C189" s="6"/>
@@ -20736,10 +20740,10 @@
       <c r="AS189" s="6"/>
     </row>
     <row r="190" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A190" s="300">
+      <c r="A190" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B190" s="300">
+      <c r="B190" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C190" s="6"/>
@@ -20787,10 +20791,10 @@
       <c r="AS190" s="6"/>
     </row>
     <row r="191" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A191" s="300">
+      <c r="A191" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B191" s="300">
+      <c r="B191" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C191" s="6"/>
@@ -20838,10 +20842,10 @@
       <c r="AS191" s="6"/>
     </row>
     <row r="192" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A192" s="300">
+      <c r="A192" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B192" s="300">
+      <c r="B192" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C192" s="6"/>
@@ -20889,10 +20893,10 @@
       <c r="AS192" s="6"/>
     </row>
     <row r="193" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A193" s="300">
+      <c r="A193" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B193" s="300">
+      <c r="B193" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C193" s="6"/>
@@ -20940,10 +20944,10 @@
       <c r="AS193" s="6"/>
     </row>
     <row r="194" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A194" s="300">
+      <c r="A194" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B194" s="300">
+      <c r="B194" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C194" s="6"/>
@@ -20991,10 +20995,10 @@
       <c r="AS194" s="6"/>
     </row>
     <row r="195" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A195" s="300">
+      <c r="A195" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B195" s="300">
+      <c r="B195" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C195" s="6"/>
@@ -21042,10 +21046,10 @@
       <c r="AS195" s="6"/>
     </row>
     <row r="196" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A196" s="300">
+      <c r="A196" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B196" s="300">
+      <c r="B196" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C196" s="6"/>
@@ -21093,10 +21097,10 @@
       <c r="AS196" s="6"/>
     </row>
     <row r="197" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A197" s="300">
+      <c r="A197" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B197" s="300">
+      <c r="B197" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C197" s="6"/>
@@ -21144,10 +21148,10 @@
       <c r="AS197" s="6"/>
     </row>
     <row r="198" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A198" s="300">
+      <c r="A198" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B198" s="300">
+      <c r="B198" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C198" s="6"/>
@@ -21195,10 +21199,10 @@
       <c r="AS198" s="6"/>
     </row>
     <row r="199" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A199" s="300">
+      <c r="A199" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B199" s="300">
+      <c r="B199" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C199" s="6"/>
@@ -21246,10 +21250,10 @@
       <c r="AS199" s="6"/>
     </row>
     <row r="200" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A200" s="300">
+      <c r="A200" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B200" s="300">
+      <c r="B200" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C200" s="6"/>
@@ -21297,10 +21301,10 @@
       <c r="AS200" s="6"/>
     </row>
     <row r="201" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A201" s="300">
+      <c r="A201" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B201" s="300">
+      <c r="B201" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C201" s="6"/>
@@ -21348,10 +21352,10 @@
       <c r="AS201" s="6"/>
     </row>
     <row r="202" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A202" s="300">
+      <c r="A202" s="288">
         <v>0.625</v>
       </c>
-      <c r="B202" s="300">
+      <c r="B202" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C202" s="6"/>
@@ -21399,10 +21403,10 @@
       <c r="AS202" s="6"/>
     </row>
     <row r="203" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A203" s="300">
+      <c r="A203" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B203" s="300">
+      <c r="B203" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C203" s="6"/>
@@ -21450,10 +21454,10 @@
       <c r="AS203" s="6"/>
     </row>
     <row r="204" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A204" s="300">
+      <c r="A204" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B204" s="300">
+      <c r="B204" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C204" s="6"/>
@@ -21501,10 +21505,10 @@
       <c r="AS204" s="6"/>
     </row>
     <row r="205" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A205" s="300">
+      <c r="A205" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B205" s="300">
+      <c r="B205" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C205" s="6"/>
@@ -21552,10 +21556,10 @@
       <c r="AS205" s="6"/>
     </row>
     <row r="206" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A206" s="300">
+      <c r="A206" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B206" s="300">
+      <c r="B206" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C206" s="6"/>
@@ -21717,25 +21721,25 @@
       </c>
       <c r="X208" s="295"/>
       <c r="AA208" s="7"/>
-      <c r="AB208" s="289" t="s">
+      <c r="AB208" s="296" t="s">
         <v>9</v>
       </c>
-      <c r="AC208" s="289"/>
+      <c r="AC208" s="296"/>
       <c r="AF208" s="7"/>
-      <c r="AG208" s="290" t="s">
+      <c r="AG208" s="298" t="s">
         <v>10</v>
       </c>
-      <c r="AH208" s="290"/>
+      <c r="AH208" s="298"/>
       <c r="AK208" s="7"/>
-      <c r="AL208" s="298" t="s">
+      <c r="AL208" s="289" t="s">
         <v>12</v>
       </c>
-      <c r="AM208" s="298"/>
+      <c r="AM208" s="289"/>
       <c r="AP208" s="7"/>
-      <c r="AQ208" s="299" t="s">
+      <c r="AQ208" s="290" t="s">
         <v>13</v>
       </c>
-      <c r="AR208" s="299"/>
+      <c r="AR208" s="290"/>
       <c r="AS208" s="7"/>
     </row>
     <row r="209" spans="1:45" s="282" customFormat="1" x14ac:dyDescent="0.15">
@@ -21745,69 +21749,69 @@
       <c r="B209" s="276"/>
       <c r="C209" s="24"/>
       <c r="D209" s="24"/>
-      <c r="E209" s="288" t="s">
+      <c r="E209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="F209" s="288"/>
+      <c r="F209" s="300"/>
       <c r="G209" s="24"/>
       <c r="H209" s="26"/>
       <c r="I209" s="26"/>
-      <c r="J209" s="288" t="s">
+      <c r="J209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="K209" s="288"/>
+      <c r="K209" s="300"/>
       <c r="L209" s="26"/>
       <c r="M209" s="24"/>
       <c r="N209" s="24"/>
-      <c r="O209" s="288" t="s">
+      <c r="O209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="P209" s="288"/>
+      <c r="P209" s="300"/>
       <c r="Q209" s="26"/>
       <c r="R209" s="26"/>
       <c r="S209" s="26"/>
-      <c r="T209" s="288" t="s">
+      <c r="T209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="U209" s="288"/>
+      <c r="U209" s="300"/>
       <c r="V209" s="26"/>
       <c r="W209" s="26"/>
       <c r="X209" s="26"/>
-      <c r="Y209" s="288" t="s">
+      <c r="Y209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="Z209" s="288"/>
+      <c r="Z209" s="300"/>
       <c r="AA209" s="26"/>
       <c r="AB209" s="26"/>
       <c r="AC209" s="26"/>
-      <c r="AD209" s="288" t="s">
+      <c r="AD209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AE209" s="288"/>
+      <c r="AE209" s="300"/>
       <c r="AF209" s="26"/>
       <c r="AG209" s="26"/>
       <c r="AH209" s="26"/>
-      <c r="AI209" s="288" t="s">
+      <c r="AI209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AJ209" s="288"/>
+      <c r="AJ209" s="300"/>
       <c r="AK209" s="26"/>
       <c r="AL209" s="24"/>
       <c r="AM209" s="24"/>
-      <c r="AN209" s="288" t="s">
+      <c r="AN209" s="300" t="s">
         <v>183</v>
       </c>
-      <c r="AO209" s="288"/>
+      <c r="AO209" s="300"/>
       <c r="AP209" s="26"/>
       <c r="AQ209" s="24"/>
       <c r="AR209" s="24"/>
       <c r="AS209" s="24"/>
     </row>
     <row r="210" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A210" s="300">
+      <c r="A210" s="288">
         <v>0.375</v>
       </c>
-      <c r="B210" s="300">
+      <c r="B210" s="288">
         <v>0.3888888888888889</v>
       </c>
       <c r="C210" s="6"/>
@@ -21855,10 +21859,10 @@
       <c r="AS210" s="6"/>
     </row>
     <row r="211" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A211" s="300">
+      <c r="A211" s="288">
         <v>0.39166666666666666</v>
       </c>
-      <c r="B211" s="300">
+      <c r="B211" s="288">
         <v>0.4055555555555555</v>
       </c>
       <c r="C211" s="6"/>
@@ -21906,10 +21910,10 @@
       <c r="AS211" s="6"/>
     </row>
     <row r="212" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A212" s="300">
+      <c r="A212" s="288">
         <v>0.40833333333333338</v>
       </c>
-      <c r="B212" s="300">
+      <c r="B212" s="288">
         <v>0.42222222222222222</v>
       </c>
       <c r="C212" s="6"/>
@@ -21957,10 +21961,10 @@
       <c r="AS212" s="6"/>
     </row>
     <row r="213" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A213" s="300">
+      <c r="A213" s="288">
         <v>0.42499999999999999</v>
       </c>
-      <c r="B213" s="300">
+      <c r="B213" s="288">
         <v>0.43888888888888888</v>
       </c>
       <c r="C213" s="6"/>
@@ -22008,10 +22012,10 @@
       <c r="AS213" s="6"/>
     </row>
     <row r="214" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A214" s="300">
+      <c r="A214" s="288">
         <v>0.44166666666666665</v>
       </c>
-      <c r="B214" s="300">
+      <c r="B214" s="288">
         <v>0.45555555555555555</v>
       </c>
       <c r="C214" s="6"/>
@@ -22059,10 +22063,10 @@
       <c r="AS214" s="6"/>
     </row>
     <row r="215" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A215" s="300">
+      <c r="A215" s="288">
         <v>0.45833333333333331</v>
       </c>
-      <c r="B215" s="300">
+      <c r="B215" s="288">
         <v>0.47222222222222227</v>
       </c>
       <c r="C215" s="6"/>
@@ -22110,10 +22114,10 @@
       <c r="AS215" s="6"/>
     </row>
     <row r="216" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A216" s="300">
+      <c r="A216" s="288">
         <v>0.47500000000000003</v>
       </c>
-      <c r="B216" s="300">
+      <c r="B216" s="288">
         <v>0.48888888888888887</v>
       </c>
       <c r="C216" s="6"/>
@@ -22161,10 +22165,10 @@
       <c r="AS216" s="6"/>
     </row>
     <row r="217" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A217" s="300">
+      <c r="A217" s="288">
         <v>0.4916666666666667</v>
       </c>
-      <c r="B217" s="300">
+      <c r="B217" s="288">
         <v>0.50555555555555554</v>
       </c>
       <c r="C217" s="6"/>
@@ -22212,10 +22216,10 @@
       <c r="AS217" s="6"/>
     </row>
     <row r="218" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A218" s="300">
+      <c r="A218" s="288">
         <v>0.5083333333333333</v>
       </c>
-      <c r="B218" s="300">
+      <c r="B218" s="288">
         <v>0.52222222222222225</v>
       </c>
       <c r="C218" s="6"/>
@@ -22263,10 +22267,10 @@
       <c r="AS218" s="6"/>
     </row>
     <row r="219" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A219" s="300">
+      <c r="A219" s="288">
         <v>0.52500000000000002</v>
       </c>
-      <c r="B219" s="300">
+      <c r="B219" s="288">
         <v>0.53888888888888886</v>
       </c>
       <c r="C219" s="6"/>
@@ -22314,10 +22318,10 @@
       <c r="AS219" s="6"/>
     </row>
     <row r="220" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A220" s="300">
+      <c r="A220" s="288">
         <v>0.54166666666666663</v>
       </c>
-      <c r="B220" s="300">
+      <c r="B220" s="288">
         <v>0.55555555555555558</v>
       </c>
       <c r="C220" s="6"/>
@@ -22365,10 +22369,10 @@
       <c r="AS220" s="6"/>
     </row>
     <row r="221" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A221" s="300">
+      <c r="A221" s="288">
         <v>0.55833333333333335</v>
       </c>
-      <c r="B221" s="300">
+      <c r="B221" s="288">
         <v>0.57222222222222219</v>
       </c>
       <c r="C221" s="6"/>
@@ -22416,10 +22420,10 @@
       <c r="AS221" s="5"/>
     </row>
     <row r="222" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A222" s="300">
+      <c r="A222" s="288">
         <v>0.57500000000000007</v>
       </c>
-      <c r="B222" s="300">
+      <c r="B222" s="288">
         <v>0.58888888888888891</v>
       </c>
       <c r="C222" s="6"/>
@@ -22467,10 +22471,10 @@
       <c r="AS222" s="5"/>
     </row>
     <row r="223" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A223" s="300">
+      <c r="A223" s="288">
         <v>0.59166666666666667</v>
       </c>
-      <c r="B223" s="300">
+      <c r="B223" s="288">
         <v>0.60555555555555551</v>
       </c>
       <c r="C223" s="6"/>
@@ -22518,10 +22522,10 @@
       <c r="AS223" s="6"/>
     </row>
     <row r="224" spans="1:45" x14ac:dyDescent="0.15">
-      <c r="A224" s="300">
+      <c r="A224" s="288">
         <v>0.60833333333333328</v>
       </c>
-      <c r="B224" s="300">
+      <c r="B224" s="288">
         <v>0.62222222222222223</v>
       </c>
       <c r="C224" s="6"/>
@@ -22569,10 +22573,10 @@
       <c r="AS224" s="6"/>
     </row>
     <row r="225" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A225" s="300">
+      <c r="A225" s="288">
         <v>0.625</v>
       </c>
-      <c r="B225" s="300">
+      <c r="B225" s="288">
         <v>0.63888888888888895</v>
       </c>
       <c r="C225" s="6"/>
@@ -22620,10 +22624,10 @@
       <c r="AS225" s="6"/>
     </row>
     <row r="226" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A226" s="300">
+      <c r="A226" s="288">
         <v>0.64166666666666672</v>
       </c>
-      <c r="B226" s="300">
+      <c r="B226" s="288">
         <v>0.65555555555555556</v>
       </c>
       <c r="C226" s="6"/>
@@ -22671,10 +22675,10 @@
       <c r="AS226" s="6"/>
     </row>
     <row r="227" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A227" s="300">
+      <c r="A227" s="288">
         <v>0.65833333333333333</v>
       </c>
-      <c r="B227" s="300">
+      <c r="B227" s="288">
         <v>0.67222222222222217</v>
       </c>
       <c r="C227" s="6"/>
@@ -22722,10 +22726,10 @@
       <c r="AS227" s="6"/>
     </row>
     <row r="228" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A228" s="300">
+      <c r="A228" s="288">
         <v>0.67499999999999993</v>
       </c>
-      <c r="B228" s="300">
+      <c r="B228" s="288">
         <v>0.68888888888888899</v>
       </c>
       <c r="C228" s="6"/>
@@ -22773,10 +22777,10 @@
       <c r="AS228" s="6"/>
     </row>
     <row r="229" spans="1:47" x14ac:dyDescent="0.15">
-      <c r="A229" s="300">
+      <c r="A229" s="288">
         <v>0.69166666666666676</v>
       </c>
-      <c r="B229" s="300">
+      <c r="B229" s="288">
         <v>0.7055555555555556</v>
       </c>
       <c r="C229" s="6"/>
@@ -23022,22 +23026,132 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="AL208:AM208"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="AQ24:AR24"/>
-    <mergeCell ref="AQ47:AR47"/>
-    <mergeCell ref="AQ70:AR70"/>
-    <mergeCell ref="AQ93:AR93"/>
-    <mergeCell ref="AQ116:AR116"/>
-    <mergeCell ref="AQ139:AR139"/>
-    <mergeCell ref="AQ162:AR162"/>
-    <mergeCell ref="AQ185:AR185"/>
-    <mergeCell ref="AQ208:AR208"/>
-    <mergeCell ref="AL116:AM116"/>
-    <mergeCell ref="AL139:AM139"/>
-    <mergeCell ref="AL162:AM162"/>
-    <mergeCell ref="AL185:AM185"/>
-    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AN209:AO209"/>
+    <mergeCell ref="AN2:AO2"/>
+    <mergeCell ref="AN25:AO25"/>
+    <mergeCell ref="AN48:AO48"/>
+    <mergeCell ref="AN71:AO71"/>
+    <mergeCell ref="AN94:AO94"/>
+    <mergeCell ref="AI117:AJ117"/>
+    <mergeCell ref="AI140:AJ140"/>
+    <mergeCell ref="AI163:AJ163"/>
+    <mergeCell ref="AI186:AJ186"/>
+    <mergeCell ref="AI209:AJ209"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AI25:AJ25"/>
+    <mergeCell ref="AI48:AJ48"/>
+    <mergeCell ref="AI71:AJ71"/>
+    <mergeCell ref="AI94:AJ94"/>
+    <mergeCell ref="Y209:Z209"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AD25:AE25"/>
+    <mergeCell ref="AD48:AE48"/>
+    <mergeCell ref="AD71:AE71"/>
+    <mergeCell ref="AD94:AE94"/>
+    <mergeCell ref="AD117:AE117"/>
+    <mergeCell ref="AD140:AE140"/>
+    <mergeCell ref="AD163:AE163"/>
+    <mergeCell ref="AD186:AE186"/>
+    <mergeCell ref="AD209:AE209"/>
+    <mergeCell ref="Y48:Z48"/>
+    <mergeCell ref="Y71:Z71"/>
+    <mergeCell ref="Y94:Z94"/>
+    <mergeCell ref="Y117:Z117"/>
+    <mergeCell ref="Y140:Z140"/>
+    <mergeCell ref="AB208:AC208"/>
+    <mergeCell ref="AB116:AC116"/>
+    <mergeCell ref="O140:P140"/>
+    <mergeCell ref="O163:P163"/>
+    <mergeCell ref="O186:P186"/>
+    <mergeCell ref="O209:P209"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="T25:U25"/>
+    <mergeCell ref="T48:U48"/>
+    <mergeCell ref="T71:U71"/>
+    <mergeCell ref="T94:U94"/>
+    <mergeCell ref="T117:U117"/>
+    <mergeCell ref="T140:U140"/>
+    <mergeCell ref="T163:U163"/>
+    <mergeCell ref="T186:U186"/>
+    <mergeCell ref="T209:U209"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="O71:P71"/>
+    <mergeCell ref="O94:P94"/>
+    <mergeCell ref="E140:F140"/>
+    <mergeCell ref="E163:F163"/>
+    <mergeCell ref="E186:F186"/>
+    <mergeCell ref="E209:F209"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J94:K94"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="J140:K140"/>
+    <mergeCell ref="J163:K163"/>
+    <mergeCell ref="J186:K186"/>
+    <mergeCell ref="J209:K209"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="AG208:AH208"/>
+    <mergeCell ref="C208:D208"/>
+    <mergeCell ref="H208:I208"/>
+    <mergeCell ref="M208:N208"/>
+    <mergeCell ref="R208:S208"/>
+    <mergeCell ref="W208:X208"/>
+    <mergeCell ref="AB162:AC162"/>
+    <mergeCell ref="AG162:AH162"/>
+    <mergeCell ref="C185:D185"/>
+    <mergeCell ref="H185:I185"/>
+    <mergeCell ref="M185:N185"/>
+    <mergeCell ref="R185:S185"/>
+    <mergeCell ref="W185:X185"/>
+    <mergeCell ref="AB185:AC185"/>
+    <mergeCell ref="AG185:AH185"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="H162:I162"/>
+    <mergeCell ref="M162:N162"/>
+    <mergeCell ref="R162:S162"/>
+    <mergeCell ref="W162:X162"/>
+    <mergeCell ref="Y163:Z163"/>
+    <mergeCell ref="Y186:Z186"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="H93:I93"/>
+    <mergeCell ref="M93:N93"/>
+    <mergeCell ref="R93:S93"/>
+    <mergeCell ref="W93:X93"/>
+    <mergeCell ref="AG116:AH116"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="H139:I139"/>
+    <mergeCell ref="M139:N139"/>
+    <mergeCell ref="R139:S139"/>
+    <mergeCell ref="W139:X139"/>
+    <mergeCell ref="AB139:AC139"/>
+    <mergeCell ref="AG139:AH139"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="M116:N116"/>
+    <mergeCell ref="R116:S116"/>
+    <mergeCell ref="W116:X116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="O117:P117"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="H47:I47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="R47:S47"/>
+    <mergeCell ref="W47:X47"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="M70:N70"/>
+    <mergeCell ref="R70:S70"/>
+    <mergeCell ref="W70:X70"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="M1:N1"/>
@@ -23062,136 +23176,26 @@
     <mergeCell ref="M24:N24"/>
     <mergeCell ref="R24:S24"/>
     <mergeCell ref="W24:X24"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="R47:S47"/>
-    <mergeCell ref="W47:X47"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="M70:N70"/>
-    <mergeCell ref="R70:S70"/>
-    <mergeCell ref="W70:X70"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="H93:I93"/>
-    <mergeCell ref="M93:N93"/>
-    <mergeCell ref="R93:S93"/>
-    <mergeCell ref="W93:X93"/>
-    <mergeCell ref="AG116:AH116"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="H139:I139"/>
-    <mergeCell ref="M139:N139"/>
-    <mergeCell ref="R139:S139"/>
-    <mergeCell ref="W139:X139"/>
-    <mergeCell ref="AB139:AC139"/>
-    <mergeCell ref="AG139:AH139"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="H116:I116"/>
-    <mergeCell ref="M116:N116"/>
-    <mergeCell ref="R116:S116"/>
-    <mergeCell ref="W116:X116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="O117:P117"/>
-    <mergeCell ref="AG208:AH208"/>
-    <mergeCell ref="C208:D208"/>
-    <mergeCell ref="H208:I208"/>
-    <mergeCell ref="M208:N208"/>
-    <mergeCell ref="R208:S208"/>
-    <mergeCell ref="W208:X208"/>
-    <mergeCell ref="AB162:AC162"/>
-    <mergeCell ref="AG162:AH162"/>
-    <mergeCell ref="C185:D185"/>
-    <mergeCell ref="H185:I185"/>
-    <mergeCell ref="M185:N185"/>
-    <mergeCell ref="R185:S185"/>
-    <mergeCell ref="W185:X185"/>
-    <mergeCell ref="AB185:AC185"/>
-    <mergeCell ref="AG185:AH185"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="H162:I162"/>
-    <mergeCell ref="M162:N162"/>
-    <mergeCell ref="R162:S162"/>
-    <mergeCell ref="W162:X162"/>
-    <mergeCell ref="Y163:Z163"/>
-    <mergeCell ref="E140:F140"/>
-    <mergeCell ref="E163:F163"/>
-    <mergeCell ref="E186:F186"/>
-    <mergeCell ref="E209:F209"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="J71:K71"/>
-    <mergeCell ref="J94:K94"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="J140:K140"/>
-    <mergeCell ref="J163:K163"/>
-    <mergeCell ref="J186:K186"/>
-    <mergeCell ref="J209:K209"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E71:F71"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="O140:P140"/>
-    <mergeCell ref="O163:P163"/>
-    <mergeCell ref="O186:P186"/>
-    <mergeCell ref="O209:P209"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="T25:U25"/>
-    <mergeCell ref="T48:U48"/>
-    <mergeCell ref="T71:U71"/>
-    <mergeCell ref="T94:U94"/>
-    <mergeCell ref="T117:U117"/>
-    <mergeCell ref="T140:U140"/>
-    <mergeCell ref="T163:U163"/>
-    <mergeCell ref="T186:U186"/>
-    <mergeCell ref="T209:U209"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="O48:P48"/>
-    <mergeCell ref="O71:P71"/>
-    <mergeCell ref="O94:P94"/>
-    <mergeCell ref="Y186:Z186"/>
-    <mergeCell ref="Y209:Z209"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AD25:AE25"/>
-    <mergeCell ref="AD48:AE48"/>
-    <mergeCell ref="AD71:AE71"/>
-    <mergeCell ref="AD94:AE94"/>
-    <mergeCell ref="AD117:AE117"/>
-    <mergeCell ref="AD140:AE140"/>
-    <mergeCell ref="AD163:AE163"/>
-    <mergeCell ref="AD186:AE186"/>
-    <mergeCell ref="AD209:AE209"/>
-    <mergeCell ref="Y48:Z48"/>
-    <mergeCell ref="Y71:Z71"/>
-    <mergeCell ref="Y94:Z94"/>
-    <mergeCell ref="Y117:Z117"/>
-    <mergeCell ref="Y140:Z140"/>
-    <mergeCell ref="AB208:AC208"/>
-    <mergeCell ref="AB116:AC116"/>
-    <mergeCell ref="AI117:AJ117"/>
-    <mergeCell ref="AI140:AJ140"/>
-    <mergeCell ref="AI163:AJ163"/>
-    <mergeCell ref="AI186:AJ186"/>
-    <mergeCell ref="AI209:AJ209"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AI25:AJ25"/>
-    <mergeCell ref="AI48:AJ48"/>
-    <mergeCell ref="AI71:AJ71"/>
-    <mergeCell ref="AI94:AJ94"/>
+    <mergeCell ref="AL208:AM208"/>
+    <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="AQ24:AR24"/>
+    <mergeCell ref="AQ47:AR47"/>
+    <mergeCell ref="AQ70:AR70"/>
+    <mergeCell ref="AQ93:AR93"/>
+    <mergeCell ref="AQ116:AR116"/>
+    <mergeCell ref="AQ139:AR139"/>
+    <mergeCell ref="AQ162:AR162"/>
+    <mergeCell ref="AQ185:AR185"/>
+    <mergeCell ref="AQ208:AR208"/>
+    <mergeCell ref="AL116:AM116"/>
+    <mergeCell ref="AL139:AM139"/>
+    <mergeCell ref="AL162:AM162"/>
+    <mergeCell ref="AL185:AM185"/>
+    <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="AN117:AO117"/>
     <mergeCell ref="AN140:AO140"/>
     <mergeCell ref="AN163:AO163"/>
     <mergeCell ref="AN186:AO186"/>
-    <mergeCell ref="AN209:AO209"/>
-    <mergeCell ref="AN2:AO2"/>
-    <mergeCell ref="AN25:AO25"/>
-    <mergeCell ref="AN48:AO48"/>
-    <mergeCell ref="AN71:AO71"/>
-    <mergeCell ref="AN94:AO94"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.55118110236220474" right="0.55118110236220474" top="0.47244094488188981" bottom="0.43307086614173229" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>

<commit_message>
Clean-up the import process
</commit_message>
<xml_diff>
--- a/files/2019-2020/Zaalschema 2019-2020 v1.xlsx
+++ b/files/2019-2020/Zaalschema 2019-2020 v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erwin/Projects/zod-zaalvoetbal/files/2019-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D851C933-F5B8-1F42-B82C-7A35F2AD894F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7061C637-7CFA-514E-97EB-3AEAEFF68A49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5620" yWindow="2160" windowWidth="32800" windowHeight="20540" tabRatio="833" firstSheet="4" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="32800" windowHeight="20540" tabRatio="833" firstSheet="4" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="O13-A" sheetId="85" r:id="rId1"/>
@@ -3093,7 +3093,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -8493,9 +8493,9 @@
   </sheetPr>
   <dimension ref="A1:AU237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F26" sqref="F26"/>
+      <selection pane="topRight" activeCell="F28" sqref="E26:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9900,12 +9900,8 @@
       <c r="D26" s="95" t="s">
         <v>99</v>
       </c>
-      <c r="E26" s="284">
-        <v>4</v>
-      </c>
-      <c r="F26" s="284">
-        <v>3</v>
-      </c>
+      <c r="E26" s="284"/>
+      <c r="F26" s="284"/>
       <c r="G26" s="8"/>
       <c r="H26" s="37"/>
       <c r="I26" s="37"/>

</xml_diff>